<commit_message>
Build site at 2022-08-26 16:06:42 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3210.xlsx
+++ b/assets/disciplinas/LOM3210.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>Ementa atual:</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>519033 - Carlos Yujiro Shigue</t>
+  </si>
+  <si>
+    <t>1176388 - Luiz Tadeu Fernandes Eleno</t>
   </si>
   <si>
     <t>Programa resumido:</t>
@@ -567,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -700,97 +703,97 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" customHeight="1">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:3">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" customHeight="1">
       <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="120" customHeight="1">
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="17" spans="1:3" ht="120" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="120" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="60" customHeight="1">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="20" spans="1:3" ht="60" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="60" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="60" customHeight="1">
+      <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="120" customHeight="1">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="120" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1">
-      <c r="B24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -952,6 +955,14 @@
       </c>
       <c r="C44" s="3" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="30" customHeight="1">
+      <c r="B45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>